<commit_message>
Inclusão de melhorias @202405091045
</commit_message>
<xml_diff>
--- a/data/peers.xlsx
+++ b/data/peers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\dash_estrategia\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Meu Drive\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FD937B-4F39-4C62-BF5A-6CD5AF2D9D8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92FBBD4C-8238-4A3E-9B88-954D65B05BB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19095" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="19410" windowHeight="15585" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Trinity" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Phoenix" sheetId="6" r:id="rId3"/>
     <sheet name="Proteus" sheetId="7" r:id="rId4"/>
     <sheet name="Nemesis" sheetId="8" r:id="rId5"/>
+    <sheet name="Persevera" sheetId="9" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Nemesis!$A$1:$C$18</definedName>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="457">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="466">
   <si>
     <t>47.562.149/0001-28</t>
   </si>
@@ -1418,6 +1419,33 @@
   </si>
   <si>
     <t>XP Corporate Top CP FIRF LP</t>
+  </si>
+  <si>
+    <t>32.041.825/0001-40</t>
+  </si>
+  <si>
+    <t>Persevera Compass Advisory FIC FIM</t>
+  </si>
+  <si>
+    <t>51.487.541/0001-27</t>
+  </si>
+  <si>
+    <t>FMX Lighthouse FIC FIM</t>
+  </si>
+  <si>
+    <t>34.400.373/0001-71</t>
+  </si>
+  <si>
+    <t>Persevera Compounder Previdenciário FIFE</t>
+  </si>
+  <si>
+    <t>PERSEVERA COMPASS ADVISORY FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO MULTIMERCADO</t>
+  </si>
+  <si>
+    <t>FMX LIGHTHOUSE FUNDO DE INVESTIMENTO EM COTAS DE FUNDOS DE INVESTIMENTO MULTIMERCADO</t>
+  </si>
+  <si>
+    <t>PERSEVERA COMPOUNDER PREVIDENCIÁRIO FUNDO DE INVESTIMENTO MULTIMERCADO</t>
   </si>
 </sst>
 </file>
@@ -1461,11 +1489,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1800,7 +1827,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
@@ -1818,7 +1845,7 @@
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1829,7 +1856,7 @@
       <c r="B2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>21</v>
       </c>
     </row>
@@ -1840,7 +1867,7 @@
       <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -1851,7 +1878,7 @@
       <c r="B4" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1862,7 +1889,7 @@
       <c r="B5" t="s">
         <v>32</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1873,7 +1900,7 @@
       <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1884,7 +1911,7 @@
       <c r="B7" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>25</v>
       </c>
     </row>
@@ -1895,12 +1922,9 @@
       <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C9" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
@@ -1927,7 +1951,7 @@
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1938,7 +1962,7 @@
       <c r="B2" t="s">
         <v>213</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1949,7 +1973,7 @@
       <c r="B3" t="s">
         <v>279</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1960,7 +1984,7 @@
       <c r="B4" t="s">
         <v>329</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1971,7 +1995,7 @@
       <c r="B5" t="s">
         <v>227</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1982,7 +2006,7 @@
       <c r="B6" t="s">
         <v>335</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2125,7 +2149,7 @@
       <c r="B19" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C19" t="s">
         <v>35</v>
       </c>
     </row>
@@ -2308,7 +2332,7 @@
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2319,7 +2343,7 @@
       <c r="B2" t="s">
         <v>155</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2330,7 +2354,7 @@
       <c r="B3" t="s">
         <v>171</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>37</v>
       </c>
     </row>
@@ -2341,7 +2365,7 @@
       <c r="B4" t="s">
         <v>209</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2352,7 +2376,7 @@
       <c r="B5" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>39</v>
       </c>
     </row>
@@ -2363,7 +2387,7 @@
       <c r="B6" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>40</v>
       </c>
     </row>
@@ -2407,7 +2431,7 @@
       <c r="B10" s="1" t="s">
         <v>345</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" t="s">
         <v>352</v>
       </c>
     </row>
@@ -2436,7 +2460,7 @@
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2447,7 +2471,7 @@
       <c r="B2" t="s">
         <v>255</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" t="s">
         <v>353</v>
       </c>
     </row>
@@ -2458,7 +2482,7 @@
       <c r="B3" t="s">
         <v>315</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" t="s">
         <v>354</v>
       </c>
     </row>
@@ -2469,7 +2493,7 @@
       <c r="B4" t="s">
         <v>199</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>355</v>
       </c>
     </row>
@@ -2480,7 +2504,7 @@
       <c r="B5" t="s">
         <v>265</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" t="s">
         <v>356</v>
       </c>
     </row>
@@ -2491,7 +2515,7 @@
       <c r="B6" t="s">
         <v>153</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>357</v>
       </c>
     </row>
@@ -3041,7 +3065,7 @@
       <c r="B56" s="1" t="s">
         <v>349</v>
       </c>
-      <c r="C56" s="3" t="s">
+      <c r="C56" t="s">
         <v>418</v>
       </c>
     </row>
@@ -3373,8 +3397,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ADE661C-9EC4-48FD-9ED1-3BBE962F1779}">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3389,7 +3413,7 @@
       <c r="B1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="1" t="s">
         <v>20</v>
       </c>
     </row>
@@ -3422,7 +3446,7 @@
       <c r="B4" t="s">
         <v>147</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" t="s">
         <v>419</v>
       </c>
     </row>
@@ -3444,7 +3468,7 @@
       <c r="B6" t="s">
         <v>313</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" t="s">
         <v>420</v>
       </c>
     </row>
@@ -3455,7 +3479,7 @@
       <c r="B7" t="s">
         <v>257</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" t="s">
         <v>421</v>
       </c>
     </row>
@@ -3510,7 +3534,7 @@
       <c r="B12" t="s">
         <v>303</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" t="s">
         <v>422</v>
       </c>
     </row>
@@ -3521,7 +3545,7 @@
       <c r="B13" t="s">
         <v>183</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" t="s">
         <v>423</v>
       </c>
     </row>
@@ -3554,7 +3578,7 @@
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="3" t="s">
+      <c r="C16" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3639,4 +3663,124 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F50F2029-81E9-45AA-B30A-D9EE565B09BE}">
+  <sheetPr>
+    <tabColor theme="4" tint="0.79998168889431442"/>
+  </sheetPr>
+  <dimension ref="A1:C9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="18.28515625" style="1" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>344</v>
+      </c>
+      <c r="B4" t="s">
+        <v>345</v>
+      </c>
+      <c r="C4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>348</v>
+      </c>
+      <c r="B5" t="s">
+        <v>349</v>
+      </c>
+      <c r="C5" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>457</v>
+      </c>
+      <c r="B7" t="s">
+        <v>463</v>
+      </c>
+      <c r="C7" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>459</v>
+      </c>
+      <c r="B8" t="s">
+        <v>464</v>
+      </c>
+      <c r="C8" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="B9" t="s">
+        <v>465</v>
+      </c>
+      <c r="C9" t="s">
+        <v>462</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
+</worksheet>
 </file>
</xml_diff>